<commit_message>
fit on GDP and labor market data
</commit_message>
<xml_diff>
--- a/data/EPNM/interim/model_parameters/labor_supply_shock.xlsx
+++ b/data/EPNM/interim/model_parameters/labor_supply_shock.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="labor_supply_shock_1" sheetId="1" state="visible" r:id="rId2"/>
@@ -125,11 +125,12 @@
     <numFmt numFmtId="165" formatCode="0"/>
     <numFmt numFmtId="166" formatCode="0.00"/>
   </numFmts>
-  <fonts count="7">
+  <fonts count="8">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -145,6 +146,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FFC9211E"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="11"/>
@@ -210,7 +218,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -219,12 +227,12 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -235,7 +243,11 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -318,24 +330,24 @@
   </sheetPr>
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="A46" activeCellId="0" sqref="A46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A25" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="M65" activeCellId="0" sqref="M65"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="4" style="0" width="16.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="22.41"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="0" width="17.67"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="0" width="21.16"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="0" width="16.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="12" min="12" style="0" width="16.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.68"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="13" min="13" style="0" width="17.67"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3037,7 +3049,7 @@
         <v>7</v>
       </c>
       <c r="F64" s="0" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G64" s="0" t="n">
         <v>0</v>
@@ -3048,17 +3060,17 @@
       <c r="I64" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="J64" s="0" t="n">
-        <v>58</v>
+      <c r="J64" s="2" t="n">
+        <v>99</v>
       </c>
       <c r="K64" s="0" t="n">
-        <v>35.25</v>
+        <v>1</v>
       </c>
       <c r="L64" s="0" t="n">
-        <v>3.25</v>
+        <v>0</v>
       </c>
       <c r="M64" s="0" t="n">
-        <v>3.578125</v>
+        <v>0</v>
       </c>
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3078,7 +3090,7 @@
         <v>6</v>
       </c>
       <c r="F65" s="0" t="n">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="G65" s="0" t="n">
         <v>0</v>
@@ -3105,7 +3117,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" firstPageNumber="1" useFirstPageNumber="true" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>
@@ -3120,11 +3132,11 @@
   </sheetPr>
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="F46" activeCellId="0" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.53515625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.55078125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
@@ -3164,7 +3176,7 @@
       <c r="B3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="2" t="n">
+      <c r="C3" s="3" t="n">
         <v>9.90853658536586</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -3187,7 +3199,7 @@
       <c r="B4" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C4" s="2" t="n">
+      <c r="C4" s="3" t="n">
         <v>9.90853658536586</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -3210,7 +3222,7 @@
       <c r="B5" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="2" t="n">
+      <c r="C5" s="3" t="n">
         <v>9.90853658536586</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -3233,7 +3245,7 @@
       <c r="B6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="2" t="n">
+      <c r="C6" s="3" t="n">
         <v>9.90853658536586</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -3256,7 +3268,7 @@
       <c r="B7" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="2" t="n">
+      <c r="C7" s="3" t="n">
         <v>13.4059667673716</v>
       </c>
       <c r="D7" s="0" t="n">
@@ -3279,7 +3291,7 @@
       <c r="B8" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C8" s="2" t="n">
+      <c r="C8" s="3" t="n">
         <v>46.9132893496701</v>
       </c>
       <c r="D8" s="0" t="n">
@@ -3302,7 +3314,7 @@
       <c r="B9" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="2" t="n">
+      <c r="C9" s="3" t="n">
         <v>47.3985759231661</v>
       </c>
       <c r="D9" s="0" t="n">
@@ -3325,7 +3337,7 @@
       <c r="B10" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C10" s="2" t="n">
+      <c r="C10" s="3" t="n">
         <v>47.3985759231661</v>
       </c>
       <c r="D10" s="0" t="n">
@@ -3348,13 +3360,13 @@
       <c r="B11" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="3" t="n">
+      <c r="C11" s="4" t="n">
         <v>17.4101669199888</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>70.9635037717293</v>
       </c>
-      <c r="E11" s="2" t="n">
+      <c r="E11" s="3" t="n">
         <v>7.63540043303393</v>
       </c>
       <c r="G11" s="0" t="n">
@@ -3371,7 +3383,7 @@
       <c r="B12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="2" t="n">
+      <c r="C12" s="3" t="n">
         <v>21.1100407558355</v>
       </c>
       <c r="D12" s="0" t="n">
@@ -3394,7 +3406,7 @@
       <c r="B13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="2" t="n">
+      <c r="C13" s="3" t="n">
         <v>21.1100407558355</v>
       </c>
       <c r="D13" s="0" t="n">
@@ -3417,7 +3429,7 @@
       <c r="B14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="2" t="n">
+      <c r="C14" s="3" t="n">
         <v>21.1100407558355</v>
       </c>
       <c r="D14" s="0" t="n">
@@ -3440,7 +3452,7 @@
       <c r="B15" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="2" t="n">
+      <c r="C15" s="3" t="n">
         <v>9.62582852255719</v>
       </c>
       <c r="D15" s="0" t="n">
@@ -3463,7 +3475,7 @@
       <c r="B16" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C16" s="2" t="n">
+      <c r="C16" s="3" t="n">
         <v>9.62582852255719</v>
       </c>
       <c r="D16" s="0" t="n">
@@ -3486,7 +3498,7 @@
       <c r="B17" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C17" s="2" t="n">
+      <c r="C17" s="3" t="n">
         <v>7.96282094031344</v>
       </c>
       <c r="D17" s="0" t="n">
@@ -3509,7 +3521,7 @@
       <c r="B18" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C18" s="2" t="n">
+      <c r="C18" s="3" t="n">
         <v>7.96282094031344</v>
       </c>
       <c r="D18" s="0" t="n">
@@ -3532,7 +3544,7 @@
       <c r="B19" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C19" s="2" t="n">
+      <c r="C19" s="3" t="n">
         <v>14.7466401194624</v>
       </c>
       <c r="D19" s="0" t="n">
@@ -3555,7 +3567,7 @@
       <c r="B20" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C20" s="2" t="n">
+      <c r="C20" s="3" t="n">
         <v>13.3058537832311</v>
       </c>
       <c r="D20" s="0" t="n">
@@ -3578,7 +3590,7 @@
       <c r="B21" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C21" s="2" t="n">
+      <c r="C21" s="3" t="n">
         <v>13.3058537832311</v>
       </c>
       <c r="D21" s="0" t="n">
@@ -3601,7 +3613,7 @@
       <c r="B22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C22" s="2" t="n">
+      <c r="C22" s="3" t="n">
         <v>1.33037694013304</v>
       </c>
       <c r="D22" s="0" t="n">
@@ -3624,7 +3636,7 @@
       <c r="B23" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C23" s="2" t="n">
+      <c r="C23" s="3" t="n">
         <v>1.33037694013304</v>
       </c>
       <c r="D23" s="0" t="n">
@@ -3633,8 +3645,8 @@
       <c r="E23" s="0" t="n">
         <v>1.1</v>
       </c>
-      <c r="H23" s="3"/>
-      <c r="J23" s="2"/>
+      <c r="H23" s="4"/>
+      <c r="J23" s="3"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -3643,7 +3655,7 @@
       <c r="B24" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C24" s="2" t="n">
+      <c r="C24" s="3" t="n">
         <v>19.3357169740309</v>
       </c>
       <c r="D24" s="0" t="n">
@@ -3652,8 +3664,8 @@
       <c r="E24" s="0" t="n">
         <v>6.38125705683101</v>
       </c>
-      <c r="H24" s="3"/>
-      <c r="J24" s="2"/>
+      <c r="H24" s="4"/>
+      <c r="J24" s="3"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -3662,17 +3674,17 @@
       <c r="B25" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C25" s="3" t="n">
+      <c r="C25" s="4" t="n">
         <v>17.4101669199888</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>70.9635037717293</v>
       </c>
-      <c r="E25" s="2" t="n">
+      <c r="E25" s="3" t="n">
         <v>7.63540043303393</v>
       </c>
-      <c r="H25" s="3"/>
-      <c r="J25" s="2"/>
+      <c r="H25" s="4"/>
+      <c r="J25" s="3"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -3687,11 +3699,11 @@
       <c r="D26" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="E26" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="3"/>
-      <c r="J26" s="2"/>
+      <c r="E26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="4"/>
+      <c r="J26" s="3"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -3706,11 +3718,11 @@
       <c r="D27" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="E27" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="4"/>
-      <c r="J27" s="2"/>
+      <c r="E27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="5"/>
+      <c r="J27" s="3"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -3725,11 +3737,11 @@
       <c r="D28" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="E28" s="2" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="4"/>
-      <c r="J28" s="2"/>
+      <c r="E28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="5"/>
+      <c r="J28" s="3"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -3738,7 +3750,7 @@
       <c r="B29" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C29" s="2" t="n">
+      <c r="C29" s="3" t="n">
         <v>7.86539089848308</v>
       </c>
       <c r="D29" s="0" t="n">
@@ -3747,8 +3759,8 @@
       <c r="E29" s="0" t="n">
         <v>7.24872812135356</v>
       </c>
-      <c r="H29" s="3"/>
-      <c r="J29" s="2"/>
+      <c r="H29" s="4"/>
+      <c r="J29" s="3"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -3763,11 +3775,11 @@
       <c r="D30" s="0" t="n">
         <v>65.6</v>
       </c>
-      <c r="E30" s="2" t="n">
+      <c r="E30" s="3" t="n">
         <v>8.19</v>
       </c>
-      <c r="H30" s="4"/>
-      <c r="J30" s="2"/>
+      <c r="H30" s="5"/>
+      <c r="J30" s="3"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -3782,11 +3794,11 @@
       <c r="D31" s="0" t="n">
         <v>65.6</v>
       </c>
-      <c r="E31" s="2" t="n">
+      <c r="E31" s="3" t="n">
         <v>8.19</v>
       </c>
-      <c r="H31" s="5"/>
-      <c r="J31" s="2"/>
+      <c r="H31" s="6"/>
+      <c r="J31" s="3"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -3801,11 +3813,11 @@
       <c r="D32" s="0" t="n">
         <v>65.6</v>
       </c>
-      <c r="E32" s="2" t="n">
+      <c r="E32" s="3" t="n">
         <v>8.19</v>
       </c>
-      <c r="H32" s="3"/>
-      <c r="J32" s="2"/>
+      <c r="H32" s="4"/>
+      <c r="J32" s="3"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -3814,7 +3826,7 @@
       <c r="B33" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C33" s="2" t="n">
+      <c r="C33" s="3" t="n">
         <v>27.683615819209</v>
       </c>
       <c r="D33" s="0" t="n">
@@ -3823,8 +3835,8 @@
       <c r="E33" s="0" t="n">
         <v>5.81468926553672</v>
       </c>
-      <c r="H33" s="3"/>
-      <c r="J33" s="2"/>
+      <c r="H33" s="4"/>
+      <c r="J33" s="3"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -3833,7 +3845,7 @@
       <c r="B34" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C34" s="2" t="n">
+      <c r="C34" s="3" t="n">
         <v>27.683615819209</v>
       </c>
       <c r="D34" s="0" t="n">
@@ -3842,7 +3854,7 @@
       <c r="E34" s="0" t="n">
         <v>5.81468926553672</v>
       </c>
-      <c r="J34" s="2"/>
+      <c r="J34" s="3"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -3851,7 +3863,7 @@
       <c r="B35" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C35" s="2" t="n">
+      <c r="C35" s="3" t="n">
         <v>0</v>
       </c>
       <c r="D35" s="0" t="n">
@@ -3860,7 +3872,7 @@
       <c r="E35" s="0" t="n">
         <v>14.6466973886329</v>
       </c>
-      <c r="J35" s="2"/>
+      <c r="J35" s="3"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -3869,7 +3881,7 @@
       <c r="B36" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C36" s="2" t="n">
+      <c r="C36" s="3" t="n">
         <v>15.3459372485921</v>
       </c>
       <c r="D36" s="0" t="n">
@@ -3878,7 +3890,7 @@
       <c r="E36" s="0" t="n">
         <v>10.8930008045052</v>
       </c>
-      <c r="J36" s="2"/>
+      <c r="J36" s="3"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -3887,7 +3899,7 @@
       <c r="B37" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C37" s="2" t="n">
+      <c r="C37" s="3" t="n">
         <v>27.683615819209</v>
       </c>
       <c r="D37" s="0" t="n">
@@ -3896,16 +3908,16 @@
       <c r="E37" s="0" t="n">
         <v>5.81468926553672</v>
       </c>
-      <c r="J37" s="2"/>
+      <c r="J37" s="3"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="6" t="n">
+      <c r="B38" s="7" t="n">
         <v>70</v>
       </c>
-      <c r="C38" s="2" t="n">
+      <c r="C38" s="3" t="n">
         <v>1.08764201252029</v>
       </c>
       <c r="D38" s="0" t="n">
@@ -3922,7 +3934,7 @@
       <c r="B39" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C39" s="2" t="n">
+      <c r="C39" s="3" t="n">
         <v>66.7481237656353</v>
       </c>
       <c r="D39" s="0" t="n">
@@ -3939,7 +3951,7 @@
       <c r="B40" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C40" s="2" t="n">
+      <c r="C40" s="3" t="n">
         <v>66.7481237656353</v>
       </c>
       <c r="D40" s="0" t="n">
@@ -3956,7 +3968,7 @@
       <c r="B41" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C41" s="2" t="n">
+      <c r="C41" s="3" t="n">
         <v>66.7481237656353</v>
       </c>
       <c r="D41" s="0" t="n">
@@ -3973,7 +3985,7 @@
       <c r="B42" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C42" s="2" t="n">
+      <c r="C42" s="3" t="n">
         <v>66.7481237656353</v>
       </c>
       <c r="D42" s="0" t="n">
@@ -3990,7 +4002,7 @@
       <c r="B43" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C43" s="2" t="n">
+      <c r="C43" s="3" t="n">
         <v>70.7180020811655</v>
       </c>
       <c r="D43" s="0" t="n">
@@ -4007,7 +4019,7 @@
       <c r="B44" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C44" s="2" t="n">
+      <c r="C44" s="3" t="n">
         <v>70.7180020811655</v>
       </c>
       <c r="D44" s="0" t="n">
@@ -4024,7 +4036,7 @@
       <c r="B45" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C45" s="2" t="n">
+      <c r="C45" s="3" t="n">
         <v>70.7180020811655</v>
       </c>
       <c r="D45" s="0" t="n">
@@ -4041,7 +4053,7 @@
       <c r="B46" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C46" s="2" t="n">
+      <c r="C46" s="3" t="n">
         <v>0</v>
       </c>
       <c r="D46" s="0" t="n">
@@ -4160,7 +4172,7 @@
       <c r="B53" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C53" s="2" t="n">
+      <c r="C53" s="3" t="n">
         <v>51.734118852459</v>
       </c>
       <c r="D53" s="0" t="n">
@@ -4177,7 +4189,7 @@
       <c r="B54" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="C54" s="2" t="n">
+      <c r="C54" s="3" t="n">
         <v>7.68277571251549</v>
       </c>
       <c r="D54" s="0" t="n">
@@ -4279,7 +4291,7 @@
       <c r="B60" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="C60" s="2" t="n">
+      <c r="C60" s="3" t="n">
         <v>9.64838255977497</v>
       </c>
       <c r="D60" s="0" t="n">
@@ -4296,7 +4308,7 @@
       <c r="B61" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="C61" s="2" t="n">
+      <c r="C61" s="3" t="n">
         <v>9.64838255977497</v>
       </c>
       <c r="D61" s="0" t="n">
@@ -4377,7 +4389,7 @@
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.7875" right="0.7875" top="1.05277777777778" bottom="1.05277777777778" header="0.7875" footer="0.7875"/>
-  <pageSetup paperSize="1" scale="100" firstPageNumber="1" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" useFirstPageNumber="false" horizontalDpi="300" verticalDpi="300" copies="1"/>
+  <pageSetup paperSize="1" scale="100" fitToWidth="1" fitToHeight="1" pageOrder="downThenOver" orientation="portrait" blackAndWhite="false" draft="false" cellComments="none" horizontalDpi="300" verticalDpi="300" copies="1"/>
   <headerFooter differentFirst="false" differentOddEven="false">
     <oddHeader>&amp;C&amp;"Times New Roman,Regular"&amp;12&amp;A</oddHeader>
     <oddFooter>&amp;C&amp;"Times New Roman,Regular"&amp;12Page &amp;P</oddFooter>

</xml_diff>

<commit_message>
tryout calibration of c_s and f_s
</commit_message>
<xml_diff>
--- a/data/EPNM/interim/model_parameters/labor_supply_shock.xlsx
+++ b/data/EPNM/interim/model_parameters/labor_supply_shock.xlsx
@@ -120,12 +120,13 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="General"/>
-    <numFmt numFmtId="165" formatCode="0"/>
-    <numFmt numFmtId="166" formatCode="0.00"/>
+    <numFmt numFmtId="165" formatCode="General"/>
+    <numFmt numFmtId="166" formatCode="0"/>
+    <numFmt numFmtId="167" formatCode="0.00"/>
   </numFmts>
-  <fonts count="8">
+  <fonts count="9">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -146,6 +147,13 @@
       <sz val="10"/>
       <name val="Arial"/>
       <family val="0"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <charset val="1"/>
     </font>
     <font>
       <sz val="10"/>
@@ -218,8 +226,12 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="9">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="165" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -227,27 +239,27 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="167" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="165" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+    <xf numFmtId="166" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -330,11 +342,11 @@
   </sheetPr>
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="E15" activeCellId="0" sqref="E15"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="L38" activeCellId="0" sqref="L38"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.41"/>
@@ -580,16 +592,20 @@
       <c r="I6" s="0" t="n">
         <v>1.33079847908745</v>
       </c>
-      <c r="J6" s="0" t="n">
+      <c r="J6" s="1" t="n">
+        <f aca="false">AVERAGE(F6,B6)</f>
         <v>6.5</v>
       </c>
-      <c r="K6" s="0" t="n">
+      <c r="K6" s="1" t="n">
+        <f aca="false">AVERAGE(G6,C6)</f>
         <v>8.5</v>
       </c>
-      <c r="L6" s="0" t="n">
+      <c r="L6" s="1" t="n">
+        <f aca="false">AVERAGE(H6,D6)</f>
         <v>82.5</v>
       </c>
-      <c r="M6" s="0" t="n">
+      <c r="M6" s="1" t="n">
+        <f aca="false">AVERAGE(I6,E6)</f>
         <v>2.66539923954373</v>
       </c>
       <c r="O6" s="0" t="n">
@@ -736,7 +752,7 @@
       <c r="O9" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="P9" s="1" t="s">
+      <c r="P9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -1502,16 +1518,16 @@
       <c r="I26" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="J26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L26" s="0" t="n">
+      <c r="J26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L26" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="M26" s="0" t="n">
+      <c r="M26" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1543,16 +1559,16 @@
       <c r="I27" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="J27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L27" s="0" t="n">
+      <c r="J27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L27" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="M27" s="0" t="n">
+      <c r="M27" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -1584,16 +1600,16 @@
       <c r="I28" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="J28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L28" s="0" t="n">
+      <c r="J28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L28" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="M28" s="0" t="n">
+      <c r="M28" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2322,21 +2338,17 @@
       <c r="I46" s="0" t="n">
         <v>2.72671568627451</v>
       </c>
-      <c r="J46" s="0" t="n">
-        <f aca="false">AVERAGE(F46,B46)</f>
-        <v>39.5</v>
-      </c>
-      <c r="K46" s="0" t="n">
-        <f aca="false">AVERAGE(G46,C46)</f>
-        <v>43.5</v>
-      </c>
-      <c r="L46" s="0" t="n">
-        <f aca="false">AVERAGE(H46,D46)</f>
-        <v>14</v>
-      </c>
-      <c r="M46" s="0" t="n">
-        <f aca="false">AVERAGE(I46,E46)</f>
-        <v>2.36335784313725</v>
+      <c r="J46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L46" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="M46" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -2736,16 +2748,16 @@
       <c r="I56" s="0" t="n">
         <v>7</v>
       </c>
-      <c r="J56" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K56" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L56" s="0" t="n">
+      <c r="J56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L56" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="M56" s="0" t="n">
+      <c r="M56" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2777,16 +2789,16 @@
       <c r="I57" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="J57" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K57" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L57" s="0" t="n">
+      <c r="J57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L57" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="M57" s="0" t="n">
+      <c r="M57" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2818,16 +2830,16 @@
       <c r="I58" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="J58" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K58" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L58" s="0" t="n">
+      <c r="J58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L58" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="M58" s="0" t="n">
+      <c r="M58" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -2859,16 +2871,16 @@
       <c r="I59" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="J59" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="K59" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="L59" s="0" t="n">
+      <c r="J59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="K59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="L59" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="M59" s="0" t="n">
+      <c r="M59" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3064,16 +3076,16 @@
       <c r="I64" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="J64" s="2" t="n">
+      <c r="J64" s="3" t="n">
         <v>99</v>
       </c>
-      <c r="K64" s="0" t="n">
+      <c r="K64" s="3" t="n">
         <v>1</v>
       </c>
-      <c r="L64" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="M64" s="0" t="n">
+      <c r="L64" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="M64" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -3140,7 +3152,7 @@
       <selection pane="topLeft" activeCell="F46" activeCellId="0" sqref="F46"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.5703125" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
@@ -3180,7 +3192,7 @@
       <c r="B3" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C3" s="3" t="n">
+      <c r="C3" s="4" t="n">
         <v>9.90853658536586</v>
       </c>
       <c r="D3" s="0" t="n">
@@ -3203,7 +3215,7 @@
       <c r="B4" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C4" s="3" t="n">
+      <c r="C4" s="4" t="n">
         <v>9.90853658536586</v>
       </c>
       <c r="D4" s="0" t="n">
@@ -3226,7 +3238,7 @@
       <c r="B5" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C5" s="3" t="n">
+      <c r="C5" s="4" t="n">
         <v>9.90853658536586</v>
       </c>
       <c r="D5" s="0" t="n">
@@ -3249,7 +3261,7 @@
       <c r="B6" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C6" s="3" t="n">
+      <c r="C6" s="4" t="n">
         <v>9.90853658536586</v>
       </c>
       <c r="D6" s="0" t="n">
@@ -3272,7 +3284,7 @@
       <c r="B7" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C7" s="3" t="n">
+      <c r="C7" s="4" t="n">
         <v>13.4059667673716</v>
       </c>
       <c r="D7" s="0" t="n">
@@ -3295,7 +3307,7 @@
       <c r="B8" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C8" s="3" t="n">
+      <c r="C8" s="4" t="n">
         <v>46.9132893496701</v>
       </c>
       <c r="D8" s="0" t="n">
@@ -3318,7 +3330,7 @@
       <c r="B9" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C9" s="3" t="n">
+      <c r="C9" s="4" t="n">
         <v>47.3985759231661</v>
       </c>
       <c r="D9" s="0" t="n">
@@ -3330,7 +3342,7 @@
       <c r="G9" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="H9" s="1" t="s">
+      <c r="H9" s="2" t="s">
         <v>14</v>
       </c>
     </row>
@@ -3341,7 +3353,7 @@
       <c r="B10" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C10" s="3" t="n">
+      <c r="C10" s="4" t="n">
         <v>47.3985759231661</v>
       </c>
       <c r="D10" s="0" t="n">
@@ -3364,13 +3376,13 @@
       <c r="B11" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C11" s="4" t="n">
+      <c r="C11" s="5" t="n">
         <v>17.4101669199888</v>
       </c>
       <c r="D11" s="0" t="n">
         <v>70.9635037717293</v>
       </c>
-      <c r="E11" s="3" t="n">
+      <c r="E11" s="4" t="n">
         <v>7.63540043303393</v>
       </c>
       <c r="G11" s="0" t="n">
@@ -3387,7 +3399,7 @@
       <c r="B12" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C12" s="3" t="n">
+      <c r="C12" s="4" t="n">
         <v>21.1100407558355</v>
       </c>
       <c r="D12" s="0" t="n">
@@ -3410,7 +3422,7 @@
       <c r="B13" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C13" s="3" t="n">
+      <c r="C13" s="4" t="n">
         <v>21.1100407558355</v>
       </c>
       <c r="D13" s="0" t="n">
@@ -3433,7 +3445,7 @@
       <c r="B14" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C14" s="3" t="n">
+      <c r="C14" s="4" t="n">
         <v>21.1100407558355</v>
       </c>
       <c r="D14" s="0" t="n">
@@ -3456,7 +3468,7 @@
       <c r="B15" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C15" s="3" t="n">
+      <c r="C15" s="4" t="n">
         <v>9.62582852255719</v>
       </c>
       <c r="D15" s="0" t="n">
@@ -3479,7 +3491,7 @@
       <c r="B16" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C16" s="3" t="n">
+      <c r="C16" s="4" t="n">
         <v>9.62582852255719</v>
       </c>
       <c r="D16" s="0" t="n">
@@ -3502,7 +3514,7 @@
       <c r="B17" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C17" s="3" t="n">
+      <c r="C17" s="4" t="n">
         <v>7.96282094031344</v>
       </c>
       <c r="D17" s="0" t="n">
@@ -3525,7 +3537,7 @@
       <c r="B18" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C18" s="3" t="n">
+      <c r="C18" s="4" t="n">
         <v>7.96282094031344</v>
       </c>
       <c r="D18" s="0" t="n">
@@ -3548,7 +3560,7 @@
       <c r="B19" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C19" s="3" t="n">
+      <c r="C19" s="4" t="n">
         <v>14.7466401194624</v>
       </c>
       <c r="D19" s="0" t="n">
@@ -3571,7 +3583,7 @@
       <c r="B20" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C20" s="3" t="n">
+      <c r="C20" s="4" t="n">
         <v>13.3058537832311</v>
       </c>
       <c r="D20" s="0" t="n">
@@ -3594,7 +3606,7 @@
       <c r="B21" s="0" t="n">
         <v>8</v>
       </c>
-      <c r="C21" s="3" t="n">
+      <c r="C21" s="4" t="n">
         <v>13.3058537832311</v>
       </c>
       <c r="D21" s="0" t="n">
@@ -3617,7 +3629,7 @@
       <c r="B22" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C22" s="3" t="n">
+      <c r="C22" s="4" t="n">
         <v>1.33037694013304</v>
       </c>
       <c r="D22" s="0" t="n">
@@ -3640,7 +3652,7 @@
       <c r="B23" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C23" s="3" t="n">
+      <c r="C23" s="4" t="n">
         <v>1.33037694013304</v>
       </c>
       <c r="D23" s="0" t="n">
@@ -3649,8 +3661,8 @@
       <c r="E23" s="0" t="n">
         <v>1.1</v>
       </c>
-      <c r="H23" s="4"/>
-      <c r="J23" s="3"/>
+      <c r="H23" s="5"/>
+      <c r="J23" s="4"/>
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
@@ -3659,7 +3671,7 @@
       <c r="B24" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C24" s="3" t="n">
+      <c r="C24" s="4" t="n">
         <v>19.3357169740309</v>
       </c>
       <c r="D24" s="0" t="n">
@@ -3668,8 +3680,8 @@
       <c r="E24" s="0" t="n">
         <v>6.38125705683101</v>
       </c>
-      <c r="H24" s="4"/>
-      <c r="J24" s="3"/>
+      <c r="H24" s="5"/>
+      <c r="J24" s="4"/>
     </row>
     <row r="25" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="0" t="n">
@@ -3678,17 +3690,17 @@
       <c r="B25" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C25" s="4" t="n">
+      <c r="C25" s="5" t="n">
         <v>17.4101669199888</v>
       </c>
       <c r="D25" s="0" t="n">
         <v>70.9635037717293</v>
       </c>
-      <c r="E25" s="3" t="n">
+      <c r="E25" s="4" t="n">
         <v>7.63540043303393</v>
       </c>
-      <c r="H25" s="4"/>
-      <c r="J25" s="3"/>
+      <c r="H25" s="5"/>
+      <c r="J25" s="4"/>
     </row>
     <row r="26" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="0" t="n">
@@ -3703,11 +3715,11 @@
       <c r="D26" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="E26" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H26" s="4"/>
-      <c r="J26" s="3"/>
+      <c r="E26" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H26" s="5"/>
+      <c r="J26" s="4"/>
     </row>
     <row r="27" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="0" t="n">
@@ -3722,11 +3734,11 @@
       <c r="D27" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="E27" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="5"/>
-      <c r="J27" s="3"/>
+      <c r="E27" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="6"/>
+      <c r="J27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
@@ -3741,11 +3753,11 @@
       <c r="D28" s="0" t="n">
         <v>100</v>
       </c>
-      <c r="E28" s="3" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="5"/>
-      <c r="J28" s="3"/>
+      <c r="E28" s="4" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="6"/>
+      <c r="J28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
@@ -3754,7 +3766,7 @@
       <c r="B29" s="0" t="n">
         <v>4</v>
       </c>
-      <c r="C29" s="3" t="n">
+      <c r="C29" s="4" t="n">
         <v>7.86539089848308</v>
       </c>
       <c r="D29" s="0" t="n">
@@ -3763,8 +3775,8 @@
       <c r="E29" s="0" t="n">
         <v>7.24872812135356</v>
       </c>
-      <c r="H29" s="4"/>
-      <c r="J29" s="3"/>
+      <c r="H29" s="5"/>
+      <c r="J29" s="4"/>
     </row>
     <row r="30" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="0" t="n">
@@ -3779,11 +3791,11 @@
       <c r="D30" s="0" t="n">
         <v>65.6</v>
       </c>
-      <c r="E30" s="3" t="n">
+      <c r="E30" s="4" t="n">
         <v>8.19</v>
       </c>
-      <c r="H30" s="5"/>
-      <c r="J30" s="3"/>
+      <c r="H30" s="6"/>
+      <c r="J30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="0" t="n">
@@ -3798,11 +3810,11 @@
       <c r="D31" s="0" t="n">
         <v>65.6</v>
       </c>
-      <c r="E31" s="3" t="n">
+      <c r="E31" s="4" t="n">
         <v>8.19</v>
       </c>
-      <c r="H31" s="6"/>
-      <c r="J31" s="3"/>
+      <c r="H31" s="7"/>
+      <c r="J31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="0" t="n">
@@ -3817,11 +3829,11 @@
       <c r="D32" s="0" t="n">
         <v>65.6</v>
       </c>
-      <c r="E32" s="3" t="n">
+      <c r="E32" s="4" t="n">
         <v>8.19</v>
       </c>
-      <c r="H32" s="4"/>
-      <c r="J32" s="3"/>
+      <c r="H32" s="5"/>
+      <c r="J32" s="4"/>
     </row>
     <row r="33" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="0" t="n">
@@ -3830,7 +3842,7 @@
       <c r="B33" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C33" s="3" t="n">
+      <c r="C33" s="4" t="n">
         <v>27.683615819209</v>
       </c>
       <c r="D33" s="0" t="n">
@@ -3839,8 +3851,8 @@
       <c r="E33" s="0" t="n">
         <v>5.81468926553672</v>
       </c>
-      <c r="H33" s="4"/>
-      <c r="J33" s="3"/>
+      <c r="H33" s="5"/>
+      <c r="J33" s="4"/>
     </row>
     <row r="34" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="0" t="n">
@@ -3849,7 +3861,7 @@
       <c r="B34" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C34" s="3" t="n">
+      <c r="C34" s="4" t="n">
         <v>27.683615819209</v>
       </c>
       <c r="D34" s="0" t="n">
@@ -3858,7 +3870,7 @@
       <c r="E34" s="0" t="n">
         <v>5.81468926553672</v>
       </c>
-      <c r="J34" s="3"/>
+      <c r="J34" s="4"/>
     </row>
     <row r="35" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="0" t="n">
@@ -3867,7 +3879,7 @@
       <c r="B35" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C35" s="3" t="n">
+      <c r="C35" s="4" t="n">
         <v>0</v>
       </c>
       <c r="D35" s="0" t="n">
@@ -3876,7 +3888,7 @@
       <c r="E35" s="0" t="n">
         <v>14.6466973886329</v>
       </c>
-      <c r="J35" s="3"/>
+      <c r="J35" s="4"/>
     </row>
     <row r="36" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="0" t="n">
@@ -3885,7 +3897,7 @@
       <c r="B36" s="0" t="n">
         <v>2</v>
       </c>
-      <c r="C36" s="3" t="n">
+      <c r="C36" s="4" t="n">
         <v>15.3459372485921</v>
       </c>
       <c r="D36" s="0" t="n">
@@ -3894,7 +3906,7 @@
       <c r="E36" s="0" t="n">
         <v>10.8930008045052</v>
       </c>
-      <c r="J36" s="3"/>
+      <c r="J36" s="4"/>
     </row>
     <row r="37" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="0" t="n">
@@ -3903,7 +3915,7 @@
       <c r="B37" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="C37" s="3" t="n">
+      <c r="C37" s="4" t="n">
         <v>27.683615819209</v>
       </c>
       <c r="D37" s="0" t="n">
@@ -3912,16 +3924,16 @@
       <c r="E37" s="0" t="n">
         <v>5.81468926553672</v>
       </c>
-      <c r="J37" s="3"/>
+      <c r="J37" s="4"/>
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
         <v>24</v>
       </c>
-      <c r="B38" s="7" t="n">
+      <c r="B38" s="8" t="n">
         <v>70</v>
       </c>
-      <c r="C38" s="3" t="n">
+      <c r="C38" s="4" t="n">
         <v>1.08764201252029</v>
       </c>
       <c r="D38" s="0" t="n">
@@ -3938,7 +3950,7 @@
       <c r="B39" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C39" s="3" t="n">
+      <c r="C39" s="4" t="n">
         <v>66.7481237656353</v>
       </c>
       <c r="D39" s="0" t="n">
@@ -3955,7 +3967,7 @@
       <c r="B40" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C40" s="3" t="n">
+      <c r="C40" s="4" t="n">
         <v>66.7481237656353</v>
       </c>
       <c r="D40" s="0" t="n">
@@ -3972,7 +3984,7 @@
       <c r="B41" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C41" s="3" t="n">
+      <c r="C41" s="4" t="n">
         <v>66.7481237656353</v>
       </c>
       <c r="D41" s="0" t="n">
@@ -3989,7 +4001,7 @@
       <c r="B42" s="0" t="n">
         <v>3</v>
       </c>
-      <c r="C42" s="3" t="n">
+      <c r="C42" s="4" t="n">
         <v>66.7481237656353</v>
       </c>
       <c r="D42" s="0" t="n">
@@ -4006,7 +4018,7 @@
       <c r="B43" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C43" s="3" t="n">
+      <c r="C43" s="4" t="n">
         <v>70.7180020811655</v>
       </c>
       <c r="D43" s="0" t="n">
@@ -4023,7 +4035,7 @@
       <c r="B44" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C44" s="3" t="n">
+      <c r="C44" s="4" t="n">
         <v>70.7180020811655</v>
       </c>
       <c r="D44" s="0" t="n">
@@ -4040,7 +4052,7 @@
       <c r="B45" s="0" t="n">
         <v>1</v>
       </c>
-      <c r="C45" s="3" t="n">
+      <c r="C45" s="4" t="n">
         <v>70.7180020811655</v>
       </c>
       <c r="D45" s="0" t="n">
@@ -4057,7 +4069,7 @@
       <c r="B46" s="0" t="n">
         <v>0</v>
       </c>
-      <c r="C46" s="3" t="n">
+      <c r="C46" s="4" t="n">
         <v>0</v>
       </c>
       <c r="D46" s="0" t="n">
@@ -4176,7 +4188,7 @@
       <c r="B53" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="C53" s="3" t="n">
+      <c r="C53" s="4" t="n">
         <v>51.734118852459</v>
       </c>
       <c r="D53" s="0" t="n">
@@ -4193,7 +4205,7 @@
       <c r="B54" s="0" t="n">
         <v>45</v>
       </c>
-      <c r="C54" s="3" t="n">
+      <c r="C54" s="4" t="n">
         <v>7.68277571251549</v>
       </c>
       <c r="D54" s="0" t="n">
@@ -4295,7 +4307,7 @@
       <c r="B60" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="C60" s="3" t="n">
+      <c r="C60" s="4" t="n">
         <v>9.64838255977497</v>
       </c>
       <c r="D60" s="0" t="n">
@@ -4312,7 +4324,7 @@
       <c r="B61" s="0" t="n">
         <v>57</v>
       </c>
-      <c r="C61" s="3" t="n">
+      <c r="C61" s="4" t="n">
         <v>9.64838255977497</v>
       </c>
       <c r="D61" s="0" t="n">

</xml_diff>

<commit_message>
adjust NACE 64 labels in all input files
</commit_message>
<xml_diff>
--- a/data/EPNM/interim/model_parameters/labor_supply_shock.xlsx
+++ b/data/EPNM/interim/model_parameters/labor_supply_shock.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="92" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="140" uniqueCount="94">
   <si>
     <t xml:space="preserve">ERMG survey 06-04-2020</t>
   </si>
@@ -56,36 +56,228 @@
     <t xml:space="preserve">01-02-03</t>
   </si>
   <si>
+    <t xml:space="preserve">A01</t>
+  </si>
+  <si>
+    <t xml:space="preserve">A02</t>
+  </si>
+  <si>
     <t xml:space="preserve">manufacturing average</t>
   </si>
   <si>
+    <t xml:space="preserve">A03</t>
+  </si>
+  <si>
+    <t xml:space="preserve">B05-09</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C10-12</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C13-15</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C16</t>
+  </si>
+  <si>
+    <t xml:space="preserve">46-47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C17</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C18</t>
+  </si>
+  <si>
+    <t xml:space="preserve">49-50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C19</t>
+  </si>
+  <si>
+    <t xml:space="preserve">69-70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C20</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C21</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C22</t>
+  </si>
+  <si>
+    <t xml:space="preserve">74-75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C23</t>
+  </si>
+  <si>
+    <t xml:space="preserve">transport average</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C24</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C25</t>
+  </si>
+  <si>
+    <t xml:space="preserve">no shock</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C26</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C27</t>
+  </si>
+  <si>
+    <t xml:space="preserve">87-88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C28</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C29</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C30</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C31-32</t>
+  </si>
+  <si>
+    <t xml:space="preserve">C33</t>
+  </si>
+  <si>
+    <t xml:space="preserve">D35</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E36</t>
+  </si>
+  <si>
+    <t xml:space="preserve">E37-39</t>
+  </si>
+  <si>
+    <t xml:space="preserve">F41-43</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G45</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G46</t>
+  </si>
+  <si>
+    <t xml:space="preserve">G47</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H49</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H50</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H51</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H52</t>
+  </si>
+  <si>
+    <t xml:space="preserve">H53</t>
+  </si>
+  <si>
+    <t xml:space="preserve">I55-56</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J58</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J59-60</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J61</t>
+  </si>
+  <si>
+    <t xml:space="preserve">J62-63</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K64</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K65</t>
+  </si>
+  <si>
+    <t xml:space="preserve">K66</t>
+  </si>
+  <si>
+    <t xml:space="preserve">L68</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M69-70</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M71</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M72</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M73</t>
+  </si>
+  <si>
+    <t xml:space="preserve">M74-75</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N77</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N78</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N79</t>
+  </si>
+  <si>
+    <t xml:space="preserve">N80-82</t>
+  </si>
+  <si>
+    <t xml:space="preserve">O84</t>
+  </si>
+  <si>
+    <t xml:space="preserve">P85</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q86</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Q87-88</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R90-92</t>
+  </si>
+  <si>
+    <t xml:space="preserve">R93</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S94</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S95</t>
+  </si>
+  <si>
+    <t xml:space="preserve">S96</t>
+  </si>
+  <si>
+    <t xml:space="preserve">T97-98</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ERMG survey 10-10-2020</t>
+  </si>
+  <si>
     <t xml:space="preserve">10-12</t>
   </si>
   <si>
     <t xml:space="preserve">13-15</t>
   </si>
   <si>
-    <t xml:space="preserve">46-47</t>
-  </si>
-  <si>
-    <t xml:space="preserve">49-50</t>
-  </si>
-  <si>
-    <t xml:space="preserve">69-70</t>
-  </si>
-  <si>
-    <t xml:space="preserve">74-75</t>
-  </si>
-  <si>
-    <t xml:space="preserve">transport average</t>
-  </si>
-  <si>
-    <t xml:space="preserve">no shock</t>
-  </si>
-  <si>
-    <t xml:space="preserve">87-88</t>
-  </si>
-  <si>
     <t xml:space="preserve">31-32</t>
   </si>
   <si>
@@ -111,9 +303,6 @@
   </si>
   <si>
     <t xml:space="preserve">97-98</t>
-  </si>
-  <si>
-    <t xml:space="preserve">ERMG survey 10-10-2020</t>
   </si>
 </sst>
 </file>
@@ -226,7 +415,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="10">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -249,6 +438,10 @@
     </xf>
     <xf numFmtId="167" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="166" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
     <xf numFmtId="167" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
@@ -342,11 +535,11 @@
   </sheetPr>
   <dimension ref="A1:P65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="B7" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="L38" activeCellId="0" sqref="L38"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A37" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C72" activeCellId="0" sqref="C72"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="6.01"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="0" width="22.41"/>
@@ -424,8 +617,8 @@
       </c>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A3" s="0" t="n">
-        <v>1</v>
+      <c r="A3" s="0" t="s">
+        <v>11</v>
       </c>
       <c r="B3" s="0" t="n">
         <v>4</v>
@@ -471,8 +664,8 @@
       </c>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A4" s="0" t="n">
-        <v>2</v>
+      <c r="A4" s="0" t="s">
+        <v>12</v>
       </c>
       <c r="B4" s="0" t="n">
         <v>4</v>
@@ -514,12 +707,12 @@
         <v>18</v>
       </c>
       <c r="P4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A5" s="0" t="n">
-        <v>3</v>
+      <c r="A5" s="0" t="s">
+        <v>14</v>
       </c>
       <c r="B5" s="0" t="n">
         <v>4</v>
@@ -566,7 +759,7 @@
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="0" t="s">
-        <v>9</v>
+        <v>15</v>
       </c>
       <c r="B6" s="0" t="n">
         <v>4</v>
@@ -617,7 +810,7 @@
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>7</v>
@@ -664,7 +857,7 @@
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>17</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>68</v>
@@ -706,12 +899,12 @@
         <v>33</v>
       </c>
       <c r="P8" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A9" s="0" t="n">
-        <v>16</v>
+      <c r="A9" s="0" t="s">
+        <v>18</v>
       </c>
       <c r="B9" s="0" t="n">
         <v>26</v>
@@ -753,12 +946,12 @@
         <v>45</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A10" s="0" t="n">
-        <v>17</v>
+      <c r="A10" s="0" t="s">
+        <v>20</v>
       </c>
       <c r="B10" s="0" t="n">
         <v>26</v>
@@ -804,8 +997,8 @@
       </c>
     </row>
     <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A11" s="0" t="n">
-        <v>18</v>
+      <c r="A11" s="0" t="s">
+        <v>21</v>
       </c>
       <c r="B11" s="0" t="n">
         <v>27.4299884467405</v>
@@ -847,12 +1040,12 @@
         <v>53</v>
       </c>
       <c r="P11" s="0" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A12" s="0" t="n">
-        <v>19</v>
+      <c r="A12" s="0" t="s">
+        <v>23</v>
       </c>
       <c r="B12" s="0" t="n">
         <v>14</v>
@@ -894,12 +1087,12 @@
         <v>71</v>
       </c>
       <c r="P12" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A13" s="0" t="n">
-        <v>20</v>
+      <c r="A13" s="0" t="s">
+        <v>25</v>
       </c>
       <c r="B13" s="0" t="n">
         <v>14</v>
@@ -941,12 +1134,12 @@
         <v>72</v>
       </c>
       <c r="P13" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A14" s="0" t="n">
-        <v>21</v>
+      <c r="A14" s="0" t="s">
+        <v>26</v>
       </c>
       <c r="B14" s="0" t="n">
         <v>14</v>
@@ -988,12 +1181,12 @@
         <v>73</v>
       </c>
       <c r="P14" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A15" s="0" t="n">
-        <v>22</v>
+      <c r="A15" s="0" t="s">
+        <v>27</v>
       </c>
       <c r="B15" s="0" t="n">
         <v>15</v>
@@ -1032,15 +1225,15 @@
         <v>12.1691308243728</v>
       </c>
       <c r="O15" s="0" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="P15" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A16" s="0" t="n">
-        <v>23</v>
+      <c r="A16" s="0" t="s">
+        <v>29</v>
       </c>
       <c r="B16" s="0" t="n">
         <v>15</v>
@@ -1082,12 +1275,12 @@
         <v>77</v>
       </c>
       <c r="P16" s="0" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A17" s="0" t="n">
-        <v>24</v>
+      <c r="A17" s="0" t="s">
+        <v>31</v>
       </c>
       <c r="B17" s="0" t="n">
         <v>12</v>
@@ -1129,12 +1322,12 @@
         <v>84</v>
       </c>
       <c r="P17" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A18" s="0" t="n">
-        <v>25</v>
+      <c r="A18" s="0" t="s">
+        <v>32</v>
       </c>
       <c r="B18" s="0" t="n">
         <v>12</v>
@@ -1176,12 +1369,12 @@
         <v>85</v>
       </c>
       <c r="P18" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A19" s="0" t="n">
-        <v>26</v>
+      <c r="A19" s="0" t="s">
+        <v>34</v>
       </c>
       <c r="B19" s="0" t="n">
         <v>13</v>
@@ -1223,12 +1416,12 @@
         <v>86</v>
       </c>
       <c r="P19" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A20" s="0" t="n">
-        <v>27</v>
+      <c r="A20" s="0" t="s">
+        <v>35</v>
       </c>
       <c r="B20" s="0" t="n">
         <v>26</v>
@@ -1267,15 +1460,15 @@
         <v>10.4676537585421</v>
       </c>
       <c r="O20" s="0" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="P20" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A21" s="0" t="n">
-        <v>28</v>
+      <c r="A21" s="0" t="s">
+        <v>37</v>
       </c>
       <c r="B21" s="0" t="n">
         <v>26</v>
@@ -1317,12 +1510,12 @@
         <v>94</v>
       </c>
       <c r="P21" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A22" s="0" t="n">
-        <v>29</v>
+      <c r="A22" s="0" t="s">
+        <v>38</v>
       </c>
       <c r="B22" s="0" t="n">
         <v>58</v>
@@ -1364,12 +1557,12 @@
         <v>95</v>
       </c>
       <c r="P22" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A23" s="0" t="n">
-        <v>30</v>
+      <c r="A23" s="0" t="s">
+        <v>39</v>
       </c>
       <c r="B23" s="0" t="n">
         <v>58</v>
@@ -1410,7 +1603,7 @@
     </row>
     <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>21</v>
+        <v>40</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>64</v>
@@ -1450,8 +1643,8 @@
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A25" s="0" t="n">
-        <v>33</v>
+      <c r="A25" s="0" t="s">
+        <v>41</v>
       </c>
       <c r="B25" s="0" t="n">
         <v>27.4299884467405</v>
@@ -1491,8 +1684,8 @@
       </c>
     </row>
     <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A26" s="0" t="n">
-        <v>35</v>
+      <c r="A26" s="0" t="s">
+        <v>42</v>
       </c>
       <c r="B26" s="0" t="n">
         <v>0</v>
@@ -1532,8 +1725,8 @@
       </c>
     </row>
     <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A27" s="0" t="n">
-        <v>36</v>
+      <c r="A27" s="0" t="s">
+        <v>43</v>
       </c>
       <c r="B27" s="0" t="n">
         <v>0</v>
@@ -1574,7 +1767,7 @@
     </row>
     <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="B28" s="0" t="n">
         <v>0</v>
@@ -1615,7 +1808,7 @@
     </row>
     <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>23</v>
+        <v>45</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>46</v>
@@ -1655,8 +1848,8 @@
       </c>
     </row>
     <row r="30" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A30" s="0" t="n">
-        <v>45</v>
+      <c r="A30" s="0" t="s">
+        <v>46</v>
       </c>
       <c r="B30" s="0" t="n">
         <v>46.33</v>
@@ -1696,8 +1889,8 @@
       </c>
     </row>
     <row r="31" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A31" s="0" t="n">
-        <v>46</v>
+      <c r="A31" s="0" t="s">
+        <v>47</v>
       </c>
       <c r="B31" s="0" t="n">
         <v>46.33</v>
@@ -1737,8 +1930,8 @@
       </c>
     </row>
     <row r="32" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A32" s="0" t="n">
-        <v>47</v>
+      <c r="A32" s="0" t="s">
+        <v>48</v>
       </c>
       <c r="B32" s="0" t="n">
         <v>46.33</v>
@@ -1778,7 +1971,7 @@
       </c>
     </row>
     <row r="33" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A33" s="0" t="n">
+      <c r="A33" s="0" t="s">
         <v>49</v>
       </c>
       <c r="B33" s="0" t="n">
@@ -1819,7 +2012,7 @@
       </c>
     </row>
     <row r="34" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A34" s="0" t="n">
+      <c r="A34" s="0" t="s">
         <v>50</v>
       </c>
       <c r="B34" s="0" t="n">
@@ -1860,7 +2053,7 @@
       </c>
     </row>
     <row r="35" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A35" s="0" t="n">
+      <c r="A35" s="0" t="s">
         <v>51</v>
       </c>
       <c r="B35" s="0" t="n">
@@ -1901,7 +2094,7 @@
       </c>
     </row>
     <row r="36" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A36" s="0" t="n">
+      <c r="A36" s="0" t="s">
         <v>52</v>
       </c>
       <c r="B36" s="0" t="n">
@@ -1942,7 +2135,7 @@
       </c>
     </row>
     <row r="37" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A37" s="0" t="n">
+      <c r="A37" s="0" t="s">
         <v>53</v>
       </c>
       <c r="B37" s="0" t="n">
@@ -1984,7 +2177,7 @@
     </row>
     <row r="38" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>24</v>
+        <v>54</v>
       </c>
       <c r="B38" s="0" t="n">
         <v>91</v>
@@ -2024,8 +2217,8 @@
       </c>
     </row>
     <row r="39" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A39" s="0" t="n">
-        <v>58</v>
+      <c r="A39" s="0" t="s">
+        <v>55</v>
       </c>
       <c r="B39" s="0" t="n">
         <v>19</v>
@@ -2066,7 +2259,7 @@
     </row>
     <row r="40" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>25</v>
+        <v>56</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>19</v>
@@ -2106,8 +2299,8 @@
       </c>
     </row>
     <row r="41" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A41" s="0" t="n">
-        <v>61</v>
+      <c r="A41" s="0" t="s">
+        <v>57</v>
       </c>
       <c r="B41" s="0" t="n">
         <v>19</v>
@@ -2148,7 +2341,7 @@
     </row>
     <row r="42" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>26</v>
+        <v>58</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>19</v>
@@ -2188,8 +2381,8 @@
       </c>
     </row>
     <row r="43" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A43" s="0" t="n">
-        <v>64</v>
+      <c r="A43" s="0" t="s">
+        <v>59</v>
       </c>
       <c r="B43" s="0" t="n">
         <v>2</v>
@@ -2229,8 +2422,8 @@
       </c>
     </row>
     <row r="44" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A44" s="0" t="n">
-        <v>65</v>
+      <c r="A44" s="0" t="s">
+        <v>60</v>
       </c>
       <c r="B44" s="0" t="n">
         <v>2</v>
@@ -2270,8 +2463,8 @@
       </c>
     </row>
     <row r="45" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A45" s="0" t="n">
-        <v>66</v>
+      <c r="A45" s="0" t="s">
+        <v>61</v>
       </c>
       <c r="B45" s="0" t="n">
         <v>2</v>
@@ -2311,8 +2504,8 @@
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A46" s="0" t="n">
-        <v>68</v>
+      <c r="A46" s="0" t="s">
+        <v>62</v>
       </c>
       <c r="B46" s="0" t="n">
         <v>38</v>
@@ -2353,7 +2546,7 @@
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>16</v>
+        <v>63</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>16</v>
@@ -2393,8 +2586,8 @@
       </c>
     </row>
     <row r="48" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A48" s="0" t="n">
-        <v>71</v>
+      <c r="A48" s="0" t="s">
+        <v>64</v>
       </c>
       <c r="B48" s="0" t="n">
         <v>16</v>
@@ -2434,8 +2627,8 @@
       </c>
     </row>
     <row r="49" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A49" s="0" t="n">
-        <v>72</v>
+      <c r="A49" s="0" t="s">
+        <v>65</v>
       </c>
       <c r="B49" s="0" t="n">
         <v>16</v>
@@ -2475,8 +2668,8 @@
       </c>
     </row>
     <row r="50" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A50" s="0" t="n">
-        <v>73</v>
+      <c r="A50" s="0" t="s">
+        <v>66</v>
       </c>
       <c r="B50" s="0" t="n">
         <v>16</v>
@@ -2517,7 +2710,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>17</v>
+        <v>67</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>16</v>
@@ -2557,8 +2750,8 @@
       </c>
     </row>
     <row r="52" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A52" s="0" t="n">
-        <v>77</v>
+      <c r="A52" s="0" t="s">
+        <v>68</v>
       </c>
       <c r="B52" s="0" t="n">
         <v>17.2028071408705</v>
@@ -2598,8 +2791,8 @@
       </c>
     </row>
     <row r="53" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A53" s="0" t="n">
-        <v>78</v>
+      <c r="A53" s="0" t="s">
+        <v>69</v>
       </c>
       <c r="B53" s="0" t="n">
         <v>15</v>
@@ -2639,8 +2832,8 @@
       </c>
     </row>
     <row r="54" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A54" s="0" t="n">
-        <v>79</v>
+      <c r="A54" s="0" t="s">
+        <v>70</v>
       </c>
       <c r="B54" s="0" t="n">
         <v>69</v>
@@ -2681,7 +2874,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>27</v>
+        <v>71</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>24</v>
@@ -2721,8 +2914,8 @@
       </c>
     </row>
     <row r="56" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A56" s="0" t="n">
-        <v>84</v>
+      <c r="A56" s="0" t="s">
+        <v>72</v>
       </c>
       <c r="B56" s="0" t="n">
         <v>16</v>
@@ -2762,8 +2955,8 @@
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A57" s="0" t="n">
-        <v>85</v>
+      <c r="A57" s="0" t="s">
+        <v>73</v>
       </c>
       <c r="B57" s="0" t="n">
         <v>0</v>
@@ -2803,8 +2996,8 @@
       </c>
     </row>
     <row r="58" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A58" s="0" t="n">
-        <v>86</v>
+      <c r="A58" s="0" t="s">
+        <v>74</v>
       </c>
       <c r="B58" s="0" t="n">
         <v>0</v>
@@ -2845,7 +3038,7 @@
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>20</v>
+        <v>75</v>
       </c>
       <c r="B59" s="0" t="n">
         <v>0</v>
@@ -2886,7 +3079,7 @@
     </row>
     <row r="60" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>28</v>
+        <v>76</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>76</v>
@@ -2926,8 +3119,8 @@
       </c>
     </row>
     <row r="61" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A61" s="0" t="n">
-        <v>93</v>
+      <c r="A61" s="0" t="s">
+        <v>77</v>
       </c>
       <c r="B61" s="0" t="n">
         <v>76</v>
@@ -2967,8 +3160,8 @@
       </c>
     </row>
     <row r="62" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A62" s="0" t="n">
-        <v>94</v>
+      <c r="A62" s="0" t="s">
+        <v>78</v>
       </c>
       <c r="B62" s="0" t="n">
         <v>0</v>
@@ -3008,8 +3201,8 @@
       </c>
     </row>
     <row r="63" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A63" s="0" t="n">
-        <v>95</v>
+      <c r="A63" s="0" t="s">
+        <v>79</v>
       </c>
       <c r="B63" s="0" t="n">
         <v>16</v>
@@ -3049,8 +3242,8 @@
       </c>
     </row>
     <row r="64" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
-      <c r="A64" s="0" t="n">
-        <v>96</v>
+      <c r="A64" s="0" t="s">
+        <v>80</v>
       </c>
       <c r="B64" s="0" t="n">
         <v>16</v>
@@ -3091,7 +3284,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>29</v>
+        <v>81</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>94</v>
@@ -3148,15 +3341,15 @@
   </sheetPr>
   <dimension ref="A1:J65"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="F46" activeCellId="0" sqref="F46"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A31" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="C69" activeCellId="0" sqref="C69"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.66015625" defaultRowHeight="12.8" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <sheetData>
     <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="B1" s="0" t="s">
-        <v>30</v>
+        <v>82</v>
       </c>
       <c r="G1" s="0" t="s">
         <v>3</v>
@@ -3228,7 +3421,7 @@
         <v>18</v>
       </c>
       <c r="H4" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3279,7 +3472,7 @@
     </row>
     <row r="7" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="0" t="s">
-        <v>12</v>
+        <v>83</v>
       </c>
       <c r="B7" s="0" t="n">
         <v>3</v>
@@ -3302,7 +3495,7 @@
     </row>
     <row r="8" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="0" t="s">
-        <v>13</v>
+        <v>84</v>
       </c>
       <c r="B8" s="0" t="n">
         <v>8</v>
@@ -3320,7 +3513,7 @@
         <v>33</v>
       </c>
       <c r="H8" s="0" t="s">
-        <v>11</v>
+        <v>13</v>
       </c>
     </row>
     <row r="9" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3343,7 +3536,7 @@
         <v>45</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>14</v>
+        <v>19</v>
       </c>
     </row>
     <row r="10" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3389,7 +3582,7 @@
         <v>53</v>
       </c>
       <c r="H11" s="0" t="s">
-        <v>15</v>
+        <v>22</v>
       </c>
     </row>
     <row r="12" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3412,7 +3605,7 @@
         <v>71</v>
       </c>
       <c r="H12" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="13" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3435,7 +3628,7 @@
         <v>72</v>
       </c>
       <c r="H13" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="14" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3458,7 +3651,7 @@
         <v>73</v>
       </c>
       <c r="H14" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="15" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3478,10 +3671,10 @@
         <v>11.6228351507377</v>
       </c>
       <c r="G15" s="0" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="H15" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="16" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3504,7 +3697,7 @@
         <v>77</v>
       </c>
       <c r="H16" s="0" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3527,7 +3720,7 @@
         <v>84</v>
       </c>
       <c r="H17" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3550,7 +3743,7 @@
         <v>85</v>
       </c>
       <c r="H18" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3573,7 +3766,7 @@
         <v>86</v>
       </c>
       <c r="H19" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3593,10 +3786,10 @@
         <v>7.13548057259713</v>
       </c>
       <c r="G20" s="0" t="s">
-        <v>20</v>
+        <v>36</v>
       </c>
       <c r="H20" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3619,7 +3812,7 @@
         <v>94</v>
       </c>
       <c r="H21" s="0" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
     </row>
     <row r="22" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3642,7 +3835,7 @@
         <v>95</v>
       </c>
       <c r="H22" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
     </row>
     <row r="23" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3666,7 +3859,7 @@
     </row>
     <row r="24" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="0" t="s">
-        <v>21</v>
+        <v>85</v>
       </c>
       <c r="B24" s="0" t="n">
         <v>6</v>
@@ -3706,16 +3899,16 @@
       <c r="A26" s="0" t="n">
         <v>35</v>
       </c>
-      <c r="B26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C26" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D26" s="0" t="n">
+      <c r="B26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C26" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D26" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="E26" s="4" t="n">
+      <c r="E26" s="6" t="n">
         <v>0</v>
       </c>
       <c r="H26" s="5"/>
@@ -3725,43 +3918,43 @@
       <c r="A27" s="0" t="n">
         <v>36</v>
       </c>
-      <c r="B27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C27" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D27" s="0" t="n">
+      <c r="B27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C27" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D27" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="E27" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H27" s="6"/>
+      <c r="E27" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H27" s="7"/>
       <c r="J27" s="4"/>
     </row>
     <row r="28" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="0" t="s">
-        <v>22</v>
-      </c>
-      <c r="B28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C28" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D28" s="0" t="n">
+        <v>86</v>
+      </c>
+      <c r="B28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C28" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D28" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="E28" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="H28" s="6"/>
+      <c r="E28" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="H28" s="7"/>
       <c r="J28" s="4"/>
     </row>
     <row r="29" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="0" t="s">
-        <v>23</v>
+        <v>87</v>
       </c>
       <c r="B29" s="0" t="n">
         <v>4</v>
@@ -3794,7 +3987,7 @@
       <c r="E30" s="4" t="n">
         <v>8.19</v>
       </c>
-      <c r="H30" s="6"/>
+      <c r="H30" s="7"/>
       <c r="J30" s="4"/>
     </row>
     <row r="31" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3813,7 +4006,7 @@
       <c r="E31" s="4" t="n">
         <v>8.19</v>
       </c>
-      <c r="H31" s="7"/>
+      <c r="H31" s="8"/>
       <c r="J31" s="4"/>
     </row>
     <row r="32" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3928,9 +4121,9 @@
     </row>
     <row r="38" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="0" t="s">
-        <v>24</v>
-      </c>
-      <c r="B38" s="8" t="n">
+        <v>88</v>
+      </c>
+      <c r="B38" s="9" t="n">
         <v>70</v>
       </c>
       <c r="C38" s="4" t="n">
@@ -3962,7 +4155,7 @@
     </row>
     <row r="40" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="0" t="s">
-        <v>25</v>
+        <v>89</v>
       </c>
       <c r="B40" s="0" t="n">
         <v>3</v>
@@ -3996,7 +4189,7 @@
     </row>
     <row r="42" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A42" s="0" t="s">
-        <v>26</v>
+        <v>90</v>
       </c>
       <c r="B42" s="0" t="n">
         <v>3</v>
@@ -4066,22 +4259,22 @@
       <c r="A46" s="0" t="n">
         <v>68</v>
       </c>
-      <c r="B46" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C46" s="4" t="n">
-        <v>0</v>
-      </c>
-      <c r="D46" s="0" t="n">
+      <c r="B46" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C46" s="6" t="n">
+        <v>0</v>
+      </c>
+      <c r="D46" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="E46" s="0" t="n">
+      <c r="E46" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="47" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="0" t="s">
-        <v>16</v>
+        <v>24</v>
       </c>
       <c r="B47" s="0" t="n">
         <v>4.5</v>
@@ -4149,7 +4342,7 @@
     </row>
     <row r="51" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="0" t="s">
-        <v>17</v>
+        <v>28</v>
       </c>
       <c r="B51" s="0" t="n">
         <v>4.5</v>
@@ -4217,7 +4410,7 @@
     </row>
     <row r="55" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="0" t="s">
-        <v>27</v>
+        <v>91</v>
       </c>
       <c r="B55" s="0" t="n">
         <v>6.5</v>
@@ -4236,33 +4429,33 @@
       <c r="A56" s="0" t="n">
         <v>84</v>
       </c>
-      <c r="B56" s="0" t="n">
-        <v>4.5</v>
-      </c>
-      <c r="C56" s="0" t="n">
-        <v>75.5</v>
-      </c>
-      <c r="D56" s="0" t="n">
-        <v>15.25</v>
-      </c>
-      <c r="E56" s="0" t="n">
-        <v>4.5</v>
+      <c r="B56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C56" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D56" s="3" t="n">
+        <v>100</v>
+      </c>
+      <c r="E56" s="3" t="n">
+        <v>0</v>
       </c>
     </row>
     <row r="57" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="0" t="n">
         <v>85</v>
       </c>
-      <c r="B57" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C57" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D57" s="0" t="n">
+      <c r="B57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C57" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D57" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="E57" s="0" t="n">
+      <c r="E57" s="3" t="n">
         <v>0</v>
       </c>
     </row>
@@ -4270,39 +4463,39 @@
       <c r="A58" s="0" t="n">
         <v>86</v>
       </c>
-      <c r="B58" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C58" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D58" s="0" t="n">
+      <c r="B58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C58" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D58" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="E58" s="0" t="n">
+      <c r="E58" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="59" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="0" t="s">
-        <v>20</v>
-      </c>
-      <c r="B59" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="C59" s="0" t="n">
-        <v>0</v>
-      </c>
-      <c r="D59" s="0" t="n">
+        <v>36</v>
+      </c>
+      <c r="B59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="C59" s="3" t="n">
+        <v>0</v>
+      </c>
+      <c r="D59" s="3" t="n">
         <v>100</v>
       </c>
-      <c r="E59" s="0" t="n">
+      <c r="E59" s="3" t="n">
         <v>0</v>
       </c>
     </row>
     <row r="60" customFormat="false" ht="13.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="0" t="s">
-        <v>28</v>
+        <v>92</v>
       </c>
       <c r="B60" s="0" t="n">
         <v>57</v>
@@ -4387,7 +4580,7 @@
     </row>
     <row r="65" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A65" s="0" t="s">
-        <v>29</v>
+        <v>93</v>
       </c>
       <c r="B65" s="0" t="n">
         <v>85</v>

</xml_diff>